<commit_message>
added parameter and data summary
</commit_message>
<xml_diff>
--- a/scripts/record_10.xlsx
+++ b/scripts/record_10.xlsx
@@ -16,18 +16,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>d. bounds</t>
+  </si>
+  <si>
+    <t>d. scales</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
   <si>
     <t>parameter</t>
   </si>
   <si>
-    <t>bounds</t>
-  </si>
-  <si>
-    <t>scales</t>
-  </si>
-  <si>
-    <t>optimised</t>
+    <t>p. bounds</t>
+  </si>
+  <si>
+    <t>p. scales</t>
+  </si>
+  <si>
+    <t>p. optimised</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>strain</t>
+  </si>
+  <si>
+    <t>stress</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>cycle</t>
+  </si>
+  <si>
+    <t>[0.0, 50.0]</t>
+  </si>
+  <si>
+    <t>[0.0, 0.5]</t>
+  </si>
+  <si>
+    <t>[0.0, 3.9e+02]</t>
+  </si>
+  <si>
+    <t>[0.0, 0.0]</t>
+  </si>
+  <si>
+    <t>[0.0, 1.0]</t>
   </si>
   <si>
     <t>n</t>
@@ -45,22 +87,22 @@
     <t>d</t>
   </si>
   <si>
-    <t>[1.0, 10.0]</t>
-  </si>
-  <si>
-    <t>[0.0, 10000.0]</t>
-  </si>
-  <si>
-    <t>[200.0, 500.0]</t>
-  </si>
-  <si>
-    <t>[0.0, 100.0]</t>
-  </si>
-  <si>
-    <t>[0, 10]</t>
-  </si>
-  <si>
-    <t>[0, 1]</t>
+    <t>[3.5, 10.5]</t>
+  </si>
+  <si>
+    <t>[1.5e+02, 4.5e+02]</t>
+  </si>
+  <si>
+    <t>[25.0, 75.0]</t>
+  </si>
+  <si>
+    <t>[1e+02, 3e+02]</t>
+  </si>
+  <si>
+    <t>[2.5, 7.5]</t>
+  </si>
+  <si>
+    <t>[0.0, 10.0]</t>
   </si>
 </sst>
 </file>
@@ -662,151 +704,151 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3969.736353913504</c:v>
+                  <c:v>210.3386149766334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4798.867895725411</c:v>
+                  <c:v>223.2653294220156</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2583.182858161216</c:v>
+                  <c:v>232.1451983464777</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>308.4855553103106</c:v>
+                  <c:v>240.5403686328063</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-171.0059382971331</c:v>
+                  <c:v>248.5337687489057</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-174.5062101538874</c:v>
+                  <c:v>256.1455444602247</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-282.4882722588804</c:v>
+                  <c:v>263.3938476631907</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-458.8232551490137</c:v>
+                  <c:v>270.2959571812147</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-590.5554055003067</c:v>
+                  <c:v>276.8683373779972</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-638.587255282268</c:v>
+                  <c:v>283.1266761539799</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-627.3388845866666</c:v>
+                  <c:v>289.0859209530142</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-596.4951355730664</c:v>
+                  <c:v>294.7603131729384</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-572.306395114339</c:v>
+                  <c:v>300.1634210238941</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-562.7970184806481</c:v>
+                  <c:v>305.3081708936639</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-564.4105540197434</c:v>
+                  <c:v>310.2068772894611</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-570.1995756890619</c:v>
+                  <c:v>314.8712714214943</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-575.049758639826</c:v>
+                  <c:v>319.3125284877154</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-577.1453126300053</c:v>
+                  <c:v>323.5412937153291</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-577.0168697895019</c:v>
+                  <c:v>327.5677072122668</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-575.9732461143462</c:v>
+                  <c:v>331.4014276799311</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-575.0321424043805</c:v>
+                  <c:v>335.0516550367346</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-574.5915128565398</c:v>
+                  <c:v>338.5271520001228</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-574.5844053927976</c:v>
+                  <c:v>341.836264672967</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-574.7709154037179</c:v>
+                  <c:v>344.9869421784006</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-574.9494397058043</c:v>
+                  <c:v>347.9867553854161</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-575.0315852479289</c:v>
+                  <c:v>350.8429147658038</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-575.021446292109</c:v>
+                  <c:v>353.5622874213685</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-574.9628568912522</c:v>
+                  <c:v>356.1514133187258</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-574.9480197015801</c:v>
+                  <c:v>358.6165207674283</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-575.2434877456544</c:v>
+                  <c:v>360.9635411756665</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-576.2260925715914</c:v>
+                  <c:v>363.1981231163344</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-577.8459504224461</c:v>
+                  <c:v>365.3256457348441</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-577.8490889133959</c:v>
+                  <c:v>367.3512315287368</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-566.1631355378563</c:v>
+                  <c:v>369.2797585278241</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-519.3094760859194</c:v>
+                  <c:v>371.1158719023549</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-340.3989193271486</c:v>
+                  <c:v>372.8639950254966</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-113.1602835143731</c:v>
+                  <c:v>374.5283400152685</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2832.881061643031</c:v>
+                  <c:v>376.1129177799445</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2648.245399442651</c:v>
+                  <c:v>377.621547589904</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-286.3816488247844</c:v>
+                  <c:v>379.0578661978513</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-679.5049370779434</c:v>
+                  <c:v>380.4253362377946</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-162.1902952763189</c:v>
+                  <c:v>381.7272562758239</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-42.88034341321372</c:v>
+                  <c:v>382.966765153736</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-2124.608016187155</c:v>
+                  <c:v>384.1468524219983</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-644.9441517244036</c:v>
+                  <c:v>385.2703646568107</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2862.843978620942</c:v>
+                  <c:v>386.3400122642378</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-814.3664175996987</c:v>
+                  <c:v>387.3583759757029</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3449.031992127961</c:v>
+                  <c:v>388.3279130355809</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-43.5084876848764</c:v>
+                  <c:v>389.8871769858835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -956,34 +998,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>33000</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>680</c:v>
+                  <c:v>0.0025</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>680</c:v>
+                  <c:v>6.8e-05</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>680</c:v>
+                  <c:v>6.8e-05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>680</c:v>
+                  <c:v>6.8e-05</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>680</c:v>
+                  <c:v>6.8e-05</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>680</c:v>
+                  <c:v>6.8e-05</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>680</c:v>
+                  <c:v>6.8e-05</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>680</c:v>
+                  <c:v>6.8e-05</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>680</c:v>
+                  <c:v>6.8e-05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1427,19 +1469,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1452,75 +1498,147 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2">
+        <v>6.660883283623221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3.472212690519946</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2">
+        <v>363.4621364717364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2">
-        <v>9009.113400251132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2">
+        <v>-158.2609353223543</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2">
-        <v>276.7063217135285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2">
-        <v>-13360.55823948247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="2">
+        <v>202.3720300123277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2">
-        <v>23.30856434224855</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2.507102890713211</v>
       </c>
     </row>
   </sheetData>
@@ -1575,7 +1693,7 @@
         <v>0.01005025125628141</v>
       </c>
       <c r="D3">
-        <v>3969.736353913504</v>
+        <v>210.3386149766334</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1589,7 +1707,7 @@
         <v>0.02010050251256281</v>
       </c>
       <c r="D4">
-        <v>4798.867895725411</v>
+        <v>223.2653294220156</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1603,7 +1721,7 @@
         <v>0.03015075376884422</v>
       </c>
       <c r="D5">
-        <v>2583.182858161216</v>
+        <v>232.1451983464777</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1617,7 +1735,7 @@
         <v>0.04020100502512563</v>
       </c>
       <c r="D6">
-        <v>308.4855553103106</v>
+        <v>240.5403686328063</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1631,7 +1749,7 @@
         <v>0.05025125628140704</v>
       </c>
       <c r="D7">
-        <v>-171.0059382971331</v>
+        <v>248.5337687489057</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1645,7 +1763,7 @@
         <v>0.06030150753768844</v>
       </c>
       <c r="D8">
-        <v>-174.5062101538874</v>
+        <v>256.1455444602247</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1659,7 +1777,7 @@
         <v>0.07035175879396985</v>
       </c>
       <c r="D9">
-        <v>-282.4882722588804</v>
+        <v>263.3938476631907</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1673,7 +1791,7 @@
         <v>0.08040201005025126</v>
       </c>
       <c r="D10">
-        <v>-458.8232551490137</v>
+        <v>270.2959571812147</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1687,7 +1805,7 @@
         <v>0.09045226130653267</v>
       </c>
       <c r="D11">
-        <v>-590.5554055003067</v>
+        <v>276.8683373779972</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1701,7 +1819,7 @@
         <v>0.1005025125628141</v>
       </c>
       <c r="D12">
-        <v>-638.587255282268</v>
+        <v>283.1266761539799</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1715,7 +1833,7 @@
         <v>0.1105527638190955</v>
       </c>
       <c r="D13">
-        <v>-627.3388845866666</v>
+        <v>289.0859209530142</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1729,7 +1847,7 @@
         <v>0.1206030150753769</v>
       </c>
       <c r="D14">
-        <v>-596.4951355730664</v>
+        <v>294.7603131729384</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1743,7 +1861,7 @@
         <v>0.1306532663316583</v>
       </c>
       <c r="D15">
-        <v>-572.306395114339</v>
+        <v>300.1634210238941</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1757,7 +1875,7 @@
         <v>0.1407035175879397</v>
       </c>
       <c r="D16">
-        <v>-562.7970184806481</v>
+        <v>305.3081708936639</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1771,7 +1889,7 @@
         <v>0.1507537688442211</v>
       </c>
       <c r="D17">
-        <v>-564.4105540197434</v>
+        <v>310.2068772894611</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1785,7 +1903,7 @@
         <v>0.1608040201005025</v>
       </c>
       <c r="D18">
-        <v>-570.1995756890619</v>
+        <v>314.8712714214943</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1799,7 +1917,7 @@
         <v>0.1708542713567839</v>
       </c>
       <c r="D19">
-        <v>-575.049758639826</v>
+        <v>319.3125284877154</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1813,7 +1931,7 @@
         <v>0.1809045226130653</v>
       </c>
       <c r="D20">
-        <v>-577.1453126300053</v>
+        <v>323.5412937153291</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1827,7 +1945,7 @@
         <v>0.1909547738693467</v>
       </c>
       <c r="D21">
-        <v>-577.0168697895019</v>
+        <v>327.5677072122668</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1841,7 +1959,7 @@
         <v>0.2010050251256282</v>
       </c>
       <c r="D22">
-        <v>-575.9732461143462</v>
+        <v>331.4014276799311</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1855,7 +1973,7 @@
         <v>0.2110552763819095</v>
       </c>
       <c r="D23">
-        <v>-575.0321424043805</v>
+        <v>335.0516550367346</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1869,7 +1987,7 @@
         <v>0.221105527638191</v>
       </c>
       <c r="D24">
-        <v>-574.5915128565398</v>
+        <v>338.5271520001228</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1883,7 +2001,7 @@
         <v>0.2311557788944724</v>
       </c>
       <c r="D25">
-        <v>-574.5844053927976</v>
+        <v>341.836264672967</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1897,7 +2015,7 @@
         <v>0.2412060301507538</v>
       </c>
       <c r="D26">
-        <v>-574.7709154037179</v>
+        <v>344.9869421784006</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1911,7 +2029,7 @@
         <v>0.2512562814070352</v>
       </c>
       <c r="D27">
-        <v>-574.9494397058043</v>
+        <v>347.9867553854161</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1925,7 +2043,7 @@
         <v>0.2613065326633166</v>
       </c>
       <c r="D28">
-        <v>-575.0315852479289</v>
+        <v>350.8429147658038</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1939,7 +2057,7 @@
         <v>0.271356783919598</v>
       </c>
       <c r="D29">
-        <v>-575.021446292109</v>
+        <v>353.5622874213685</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1953,7 +2071,7 @@
         <v>0.2814070351758794</v>
       </c>
       <c r="D30">
-        <v>-574.9628568912522</v>
+        <v>356.1514133187258</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1967,7 +2085,7 @@
         <v>0.2914572864321608</v>
       </c>
       <c r="D31">
-        <v>-574.9480197015801</v>
+        <v>358.6165207674283</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1981,7 +2099,7 @@
         <v>0.3015075376884422</v>
       </c>
       <c r="D32">
-        <v>-575.2434877456544</v>
+        <v>360.9635411756665</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1995,7 +2113,7 @@
         <v>0.3115577889447236</v>
       </c>
       <c r="D33">
-        <v>-576.2260925715914</v>
+        <v>363.1981231163344</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2009,7 +2127,7 @@
         <v>0.321608040201005</v>
       </c>
       <c r="D34">
-        <v>-577.8459504224461</v>
+        <v>365.3256457348441</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2023,7 +2141,7 @@
         <v>0.3316582914572864</v>
       </c>
       <c r="D35">
-        <v>-577.8490889133959</v>
+        <v>367.3512315287368</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2037,7 +2155,7 @@
         <v>0.3417085427135678</v>
       </c>
       <c r="D36">
-        <v>-566.1631355378563</v>
+        <v>369.2797585278241</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2051,7 +2169,7 @@
         <v>0.3517587939698493</v>
       </c>
       <c r="D37">
-        <v>-519.3094760859194</v>
+        <v>371.1158719023549</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2065,7 +2183,7 @@
         <v>0.3618090452261307</v>
       </c>
       <c r="D38">
-        <v>-340.3989193271486</v>
+        <v>372.8639950254966</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2079,7 +2197,7 @@
         <v>0.3718592964824121</v>
       </c>
       <c r="D39">
-        <v>-113.1602835143731</v>
+        <v>374.5283400152685</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2093,7 +2211,7 @@
         <v>0.3819095477386935</v>
       </c>
       <c r="D40">
-        <v>2832.881061643031</v>
+        <v>376.1129177799445</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2107,7 +2225,7 @@
         <v>0.3919597989949749</v>
       </c>
       <c r="D41">
-        <v>2648.245399442651</v>
+        <v>377.621547589904</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2121,7 +2239,7 @@
         <v>0.4020100502512563</v>
       </c>
       <c r="D42">
-        <v>-286.3816488247844</v>
+        <v>379.0578661978513</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2135,7 +2253,7 @@
         <v>0.4120603015075377</v>
       </c>
       <c r="D43">
-        <v>-679.5049370779434</v>
+        <v>380.4253362377946</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2149,7 +2267,7 @@
         <v>0.4221105527638191</v>
       </c>
       <c r="D44">
-        <v>-162.1902952763189</v>
+        <v>381.7272562758239</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2163,7 +2281,7 @@
         <v>0.4321608040201005</v>
       </c>
       <c r="D45">
-        <v>-42.88034341321372</v>
+        <v>382.966765153736</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2177,7 +2295,7 @@
         <v>0.4422110552763819</v>
       </c>
       <c r="D46">
-        <v>-2124.608016187155</v>
+        <v>384.1468524219983</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2191,7 +2309,7 @@
         <v>0.4522613065326633</v>
       </c>
       <c r="D47">
-        <v>-644.9441517244036</v>
+        <v>385.2703646568107</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2205,7 +2323,7 @@
         <v>0.4623115577889447</v>
       </c>
       <c r="D48">
-        <v>2862.843978620942</v>
+        <v>386.3400122642378</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2219,7 +2337,7 @@
         <v>0.4723618090452261</v>
       </c>
       <c r="D49">
-        <v>-814.3664175996987</v>
+        <v>387.3583759757029</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2233,7 +2351,7 @@
         <v>0.4824120603015075</v>
       </c>
       <c r="D50">
-        <v>3449.031992127961</v>
+        <v>388.3279130355809</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2247,7 +2365,7 @@
         <v>0.5</v>
       </c>
       <c r="D51">
-        <v>-43.5084876848764</v>
+        <v>389.8871769858835</v>
       </c>
     </row>
   </sheetData>
@@ -2277,7 +2395,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>33000</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2285,7 +2403,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>680</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2293,7 +2411,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>680</v>
+        <v>6.8E-05</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2301,7 +2419,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>680</v>
+        <v>6.8E-05</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2309,7 +2427,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>680</v>
+        <v>6.8E-05</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2317,7 +2435,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>680</v>
+        <v>6.8E-05</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2325,7 +2443,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>680</v>
+        <v>6.8E-05</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2333,7 +2451,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>680</v>
+        <v>6.8E-05</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2341,7 +2459,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>680</v>
+        <v>6.8E-05</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2349,7 +2467,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>680</v>
+        <v>6.8E-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>